<commit_message>
Minor edits for name continuity
</commit_message>
<xml_diff>
--- a/MSc_data/Data_new/BenthicCover_BlankSheet_CA.xlsx
+++ b/MSc_data/Data_new/BenthicCover_BlankSheet_CA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Desktop\MSc\Thesis\MSc_data\Data_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Desktop\MSc\Thesis\kelp_comms_2022\MSc_data\Data_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65627D94-C288-4C92-9287-0ECB4AE80370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25A0BAD-8F1D-4BAD-AEB1-4C0AE502C9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AEE024E6-ED02-4460-8513-1C7CB077737A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AEE024E6-ED02-4460-8513-1C7CB077737A}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw cover" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>SiteName</t>
   </si>
@@ -128,42 +128,15 @@
     <t>10_MacrocystisPyrifera</t>
   </si>
   <si>
-    <t>11_NereocystisLuekeana</t>
-  </si>
-  <si>
     <t>12_EgregiaMenziesii</t>
   </si>
   <si>
     <t>13_AlariaMarginata</t>
   </si>
   <si>
-    <t>18_UnknownBrown</t>
-  </si>
-  <si>
-    <t>19_CorallineStanding</t>
-  </si>
-  <si>
-    <t>20_CorallineCrustose</t>
-  </si>
-  <si>
-    <t>21_ChondracanthusExasperatus</t>
-  </si>
-  <si>
-    <t>22_UnknownRed</t>
-  </si>
-  <si>
     <t>14_LaminariaSetchellii</t>
   </si>
   <si>
-    <t>23_UlvaLactuca</t>
-  </si>
-  <si>
-    <t>13_AgarumClathratum</t>
-  </si>
-  <si>
-    <t>_NeoagarumFibriatum</t>
-  </si>
-  <si>
     <t>14_SaccharinaLatissima</t>
   </si>
   <si>
@@ -173,15 +146,6 @@
     <t>10_SargassumMuticum</t>
   </si>
   <si>
-    <t>_HaplogloiaAndersonii</t>
-  </si>
-  <si>
-    <t>24_UnknownGreen</t>
-  </si>
-  <si>
-    <t>25_TurfAlgae</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -197,9 +161,6 @@
     <t>4 to 7</t>
   </si>
   <si>
-    <t>9 to 25</t>
-  </si>
-  <si>
     <t>Benthic sediment types by size class (Wentworth scale)</t>
   </si>
   <si>
@@ -213,6 +174,51 @@
   </si>
   <si>
     <t>Name of image as saved online</t>
+  </si>
+  <si>
+    <t>11_NereocystisLuetkeana</t>
+  </si>
+  <si>
+    <t>13_AgarumSpp</t>
+  </si>
+  <si>
+    <t>18_HaplogloiaAndersonii</t>
+  </si>
+  <si>
+    <t>19_UnknownBrown</t>
+  </si>
+  <si>
+    <t>20_CorallineStanding</t>
+  </si>
+  <si>
+    <t>21_CorallineCrustose</t>
+  </si>
+  <si>
+    <t>22_ChondracanthusExasperatus</t>
+  </si>
+  <si>
+    <t>23_UnknownRed</t>
+  </si>
+  <si>
+    <t>24_UlvaLactuca</t>
+  </si>
+  <si>
+    <t>25_UnknownGreen</t>
+  </si>
+  <si>
+    <t>26_TurfAlgaeMix</t>
+  </si>
+  <si>
+    <t>Ab_CucumariaMiniata</t>
+  </si>
+  <si>
+    <t>Ab_</t>
+  </si>
+  <si>
+    <t>9 to 26</t>
+  </si>
+  <si>
+    <t>Counted adundance of an animal species</t>
   </si>
 </sst>
 </file>
@@ -256,10 +262,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,15 +581,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C35883-A3EF-41F5-AAA8-19EBB5913684}">
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -638,86 +645,90 @@
         <v>28</v>
       </c>
       <c r="S1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="T1" t="s">
         <v>29</v>
       </c>
       <c r="U1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" t="s">
-        <v>38</v>
-      </c>
       <c r="Y1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="Z1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="AA1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="AB1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="AD1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="AE1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="AF1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="AG1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="AH1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="AI1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="AJ1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>48</v>
-      </c>
+      <c r="AO1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8556558D-9353-403F-B65C-10BB2F3DDB3F}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +770,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,7 +813,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -810,7 +821,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -818,31 +829,39 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>